<commit_message>
Adding observation; correcting file name; updating help
</commit_message>
<xml_diff>
--- a/data/auralObservations.xlsx
+++ b/data/auralObservations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\code\auralLandscapes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF0F201-1653-473C-A25C-40A96D90BE5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C92EFB-5F84-4EAC-B7C3-B7A7EE7A898D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="138">
   <si>
     <t>taxon</t>
   </si>
@@ -830,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830C5A1-1504-4FB4-98E5-D787D6C4A5A6}">
-  <dimension ref="A1:K336"/>
+  <dimension ref="A1:K337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J338" sqref="J338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8531,6 +8531,26 @@
       </c>
       <c r="F336" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A337" t="s">
+        <v>10</v>
+      </c>
+      <c r="B337" t="s">
+        <v>19</v>
+      </c>
+      <c r="C337" s="2">
+        <v>44429</v>
+      </c>
+      <c r="D337" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F337" t="s">
+        <v>111</v>
+      </c>
+      <c r="J337" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating observations Now done with 2019 Botanists Field Notes
</commit_message>
<xml_diff>
--- a/data/auralObservations.xlsx
+++ b/data/auralObservations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\code\auralLandscapes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C92EFB-5F84-4EAC-B7C3-B7A7EE7A898D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C386E6F6-BFD2-47DC-BEC2-2C38DAF3EC73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="158">
   <si>
     <t>taxon</t>
   </si>
@@ -443,6 +443,66 @@
   </si>
   <si>
     <t>time inferred: evening, just after dark, backyard</t>
+  </si>
+  <si>
+    <t>approximate: "12 hours after thunderstorm"</t>
+  </si>
+  <si>
+    <t>guessing at time: walking with brooklyn on our walk around the block, which I assume was our morning walk.</t>
+  </si>
+  <si>
+    <t>guessing at time: morning, and it would have been b/f work</t>
+  </si>
+  <si>
+    <t>guessing at time: morning ride into work, and I recall the morning, and I don't think I was particularly early into work</t>
+  </si>
+  <si>
+    <t>guessing at time: evening walk with Rachel, and it was light enough to see Carex davisii</t>
+  </si>
+  <si>
+    <t>cicada</t>
+  </si>
+  <si>
+    <t>guessing at time: "late afternoon"</t>
+  </si>
+  <si>
+    <t>"just after sunrise"</t>
+  </si>
+  <si>
+    <t>crickets</t>
+  </si>
+  <si>
+    <t>Mays Lake</t>
+  </si>
+  <si>
+    <t>guessing at time: ride into work</t>
+  </si>
+  <si>
+    <t>Lillstreet art center</t>
+  </si>
+  <si>
+    <t>guessing at time: it was getting dark out, but I recall that we could still see a bit</t>
+  </si>
+  <si>
+    <t>guessing at time: it was a report from Robb Telfer</t>
+  </si>
+  <si>
+    <t>guessing at time: bike ride in</t>
+  </si>
+  <si>
+    <t>bracketing time -- "spring peepers were singing all day"</t>
+  </si>
+  <si>
+    <t>junco</t>
+  </si>
+  <si>
+    <t>guessing at time: afternoon</t>
+  </si>
+  <si>
+    <t>an hour b/f sunset</t>
+  </si>
+  <si>
+    <t>guessing at time -- morning walk w/ dog on a Saturday</t>
   </si>
 </sst>
 </file>
@@ -830,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830C5A1-1504-4FB4-98E5-D787D6C4A5A6}">
-  <dimension ref="A1:K337"/>
+  <dimension ref="A1:K383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J338" sqref="J338"/>
+    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H382" sqref="H382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8533,7 +8593,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A337" t="s">
         <v>10</v>
       </c>
@@ -8551,6 +8611,872 @@
       </c>
       <c r="J337" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="338" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A338" t="s">
+        <v>11</v>
+      </c>
+      <c r="B338" t="s">
+        <v>19</v>
+      </c>
+      <c r="C338" s="2">
+        <v>43639</v>
+      </c>
+      <c r="D338" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F338" t="s">
+        <v>26</v>
+      </c>
+      <c r="K338" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="339" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A339" t="s">
+        <v>58</v>
+      </c>
+      <c r="B339" t="s">
+        <v>47</v>
+      </c>
+      <c r="C339" s="2">
+        <v>43631</v>
+      </c>
+      <c r="D339" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F339" t="s">
+        <v>111</v>
+      </c>
+      <c r="K339" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="340" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A340" t="s">
+        <v>71</v>
+      </c>
+      <c r="B340" t="s">
+        <v>19</v>
+      </c>
+      <c r="C340" s="2">
+        <v>43633</v>
+      </c>
+      <c r="D340" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F340" t="s">
+        <v>26</v>
+      </c>
+      <c r="K340" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="341" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A341" t="s">
+        <v>84</v>
+      </c>
+      <c r="B341" t="s">
+        <v>19</v>
+      </c>
+      <c r="C341" s="2">
+        <v>43633</v>
+      </c>
+      <c r="D341" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F341" t="s">
+        <v>26</v>
+      </c>
+      <c r="K341" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="342" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A342" t="s">
+        <v>72</v>
+      </c>
+      <c r="B342" t="s">
+        <v>19</v>
+      </c>
+      <c r="C342" s="2">
+        <v>43633</v>
+      </c>
+      <c r="D342" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F342" t="s">
+        <v>26</v>
+      </c>
+      <c r="K342" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A343" t="s">
+        <v>32</v>
+      </c>
+      <c r="B343" t="s">
+        <v>19</v>
+      </c>
+      <c r="C343" s="2">
+        <v>43633</v>
+      </c>
+      <c r="D343" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F343" t="s">
+        <v>26</v>
+      </c>
+      <c r="K343" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A344" t="s">
+        <v>75</v>
+      </c>
+      <c r="B344" t="s">
+        <v>19</v>
+      </c>
+      <c r="C344" s="2">
+        <v>43633</v>
+      </c>
+      <c r="D344" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F344" t="s">
+        <v>26</v>
+      </c>
+      <c r="K344" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A345" t="s">
+        <v>75</v>
+      </c>
+      <c r="B345" t="s">
+        <v>19</v>
+      </c>
+      <c r="C345" s="2">
+        <v>43623</v>
+      </c>
+      <c r="D345" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F345" t="s">
+        <v>40</v>
+      </c>
+      <c r="K345" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A346" t="s">
+        <v>72</v>
+      </c>
+      <c r="B346" t="s">
+        <v>19</v>
+      </c>
+      <c r="C346" s="2">
+        <v>43623</v>
+      </c>
+      <c r="D346" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F346" t="s">
+        <v>40</v>
+      </c>
+      <c r="K346" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="347" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A347" t="s">
+        <v>71</v>
+      </c>
+      <c r="B347" t="s">
+        <v>19</v>
+      </c>
+      <c r="C347" s="2">
+        <v>43623</v>
+      </c>
+      <c r="D347" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F347" t="s">
+        <v>40</v>
+      </c>
+      <c r="K347" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="348" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A348" t="s">
+        <v>11</v>
+      </c>
+      <c r="B348" t="s">
+        <v>19</v>
+      </c>
+      <c r="C348" s="2">
+        <v>43630</v>
+      </c>
+      <c r="D348" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F348" t="s">
+        <v>26</v>
+      </c>
+      <c r="K348" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A349" t="s">
+        <v>143</v>
+      </c>
+      <c r="B349" t="s">
+        <v>22</v>
+      </c>
+      <c r="C349" s="2">
+        <v>43647</v>
+      </c>
+      <c r="D349" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F349" t="s">
+        <v>111</v>
+      </c>
+      <c r="K349" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A350" t="s">
+        <v>72</v>
+      </c>
+      <c r="B350" t="s">
+        <v>19</v>
+      </c>
+      <c r="C350" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D350" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F350" t="s">
+        <v>40</v>
+      </c>
+      <c r="K350" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A351" t="s">
+        <v>92</v>
+      </c>
+      <c r="B351" t="s">
+        <v>19</v>
+      </c>
+      <c r="C351" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D351" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F351" t="s">
+        <v>40</v>
+      </c>
+      <c r="K351" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A352" t="s">
+        <v>7</v>
+      </c>
+      <c r="B352" t="s">
+        <v>19</v>
+      </c>
+      <c r="C352" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D352" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F352" t="s">
+        <v>40</v>
+      </c>
+      <c r="K352" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A353" t="s">
+        <v>12</v>
+      </c>
+      <c r="B353" t="s">
+        <v>19</v>
+      </c>
+      <c r="C353" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D353" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F353" t="s">
+        <v>40</v>
+      </c>
+      <c r="K353" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A354" t="s">
+        <v>71</v>
+      </c>
+      <c r="B354" t="s">
+        <v>19</v>
+      </c>
+      <c r="C354" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D354" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F354" t="s">
+        <v>40</v>
+      </c>
+      <c r="K354" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A355" t="s">
+        <v>16</v>
+      </c>
+      <c r="B355" t="s">
+        <v>19</v>
+      </c>
+      <c r="C355" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D355" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F355" t="s">
+        <v>40</v>
+      </c>
+      <c r="K355" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A356" t="s">
+        <v>59</v>
+      </c>
+      <c r="B356" t="s">
+        <v>19</v>
+      </c>
+      <c r="C356" s="2">
+        <v>43648</v>
+      </c>
+      <c r="D356" s="3">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F356" t="s">
+        <v>40</v>
+      </c>
+      <c r="K356" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="357" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A357" t="s">
+        <v>16</v>
+      </c>
+      <c r="B357" t="s">
+        <v>19</v>
+      </c>
+      <c r="C357" s="2">
+        <v>43697</v>
+      </c>
+      <c r="D357" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F357" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A358" t="s">
+        <v>72</v>
+      </c>
+      <c r="B358" t="s">
+        <v>19</v>
+      </c>
+      <c r="C358" s="2">
+        <v>43697</v>
+      </c>
+      <c r="D358" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="F358" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A359" t="s">
+        <v>146</v>
+      </c>
+      <c r="B359" t="s">
+        <v>22</v>
+      </c>
+      <c r="C359" s="2">
+        <v>43697</v>
+      </c>
+      <c r="D359" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F359" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A360" t="s">
+        <v>143</v>
+      </c>
+      <c r="B360" t="s">
+        <v>22</v>
+      </c>
+      <c r="C360" s="2">
+        <v>43697</v>
+      </c>
+      <c r="D360" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F360" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A361" t="s">
+        <v>72</v>
+      </c>
+      <c r="B361" t="s">
+        <v>19</v>
+      </c>
+      <c r="C361" s="2">
+        <v>43697</v>
+      </c>
+      <c r="D361" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F361" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A362" t="s">
+        <v>146</v>
+      </c>
+      <c r="B362" t="s">
+        <v>22</v>
+      </c>
+      <c r="C362" s="2">
+        <v>43700</v>
+      </c>
+      <c r="D362" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F362" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A363" t="s">
+        <v>87</v>
+      </c>
+      <c r="B363" t="s">
+        <v>19</v>
+      </c>
+      <c r="C363" s="2">
+        <v>43700</v>
+      </c>
+      <c r="D363" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F363" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A364" t="s">
+        <v>33</v>
+      </c>
+      <c r="B364" t="s">
+        <v>19</v>
+      </c>
+      <c r="C364" s="2">
+        <v>43736</v>
+      </c>
+      <c r="D364" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F364" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A365" t="s">
+        <v>72</v>
+      </c>
+      <c r="B365" t="s">
+        <v>19</v>
+      </c>
+      <c r="C365" s="2">
+        <v>43721</v>
+      </c>
+      <c r="D365" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F365" t="s">
+        <v>40</v>
+      </c>
+      <c r="K365" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A366" t="s">
+        <v>146</v>
+      </c>
+      <c r="B366" t="s">
+        <v>22</v>
+      </c>
+      <c r="C366" s="2">
+        <v>43721</v>
+      </c>
+      <c r="D366" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F366" t="s">
+        <v>40</v>
+      </c>
+      <c r="K366" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A367" t="s">
+        <v>21</v>
+      </c>
+      <c r="B367" t="s">
+        <v>22</v>
+      </c>
+      <c r="C367" s="2">
+        <v>43722</v>
+      </c>
+      <c r="D367" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F367" t="s">
+        <v>149</v>
+      </c>
+      <c r="K367" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A368" t="s">
+        <v>51</v>
+      </c>
+      <c r="B368" t="s">
+        <v>19</v>
+      </c>
+      <c r="C368" s="2">
+        <v>43755</v>
+      </c>
+      <c r="D368" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F368" t="s">
+        <v>40</v>
+      </c>
+      <c r="K368" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A369" t="s">
+        <v>146</v>
+      </c>
+      <c r="C369" s="2">
+        <v>43738</v>
+      </c>
+      <c r="D369" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F369" t="s">
+        <v>40</v>
+      </c>
+      <c r="K369" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A370" t="s">
+        <v>50</v>
+      </c>
+      <c r="B370" t="s">
+        <v>47</v>
+      </c>
+      <c r="C370" s="2">
+        <v>43738</v>
+      </c>
+      <c r="D370" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F370" t="s">
+        <v>40</v>
+      </c>
+      <c r="K370" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A371" t="s">
+        <v>50</v>
+      </c>
+      <c r="B371" t="s">
+        <v>47</v>
+      </c>
+      <c r="C371" s="2">
+        <v>43738</v>
+      </c>
+      <c r="D371" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F371" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A372" t="s">
+        <v>50</v>
+      </c>
+      <c r="B372" t="s">
+        <v>47</v>
+      </c>
+      <c r="C372" s="2">
+        <v>43740</v>
+      </c>
+      <c r="D372" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F372" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A373" t="s">
+        <v>51</v>
+      </c>
+      <c r="B373" t="s">
+        <v>19</v>
+      </c>
+      <c r="C373" s="2">
+        <v>43770</v>
+      </c>
+      <c r="D373" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F373" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A374" t="s">
+        <v>154</v>
+      </c>
+      <c r="B374" t="s">
+        <v>19</v>
+      </c>
+      <c r="C374" s="2">
+        <v>43770</v>
+      </c>
+      <c r="D374" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F374" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A375" t="s">
+        <v>7</v>
+      </c>
+      <c r="B375" t="s">
+        <v>19</v>
+      </c>
+      <c r="C375" s="2">
+        <v>43770</v>
+      </c>
+      <c r="D375" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F375" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A376" t="s">
+        <v>11</v>
+      </c>
+      <c r="B376" t="s">
+        <v>19</v>
+      </c>
+      <c r="C376" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D376" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F376" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A377" t="s">
+        <v>101</v>
+      </c>
+      <c r="B377" t="s">
+        <v>19</v>
+      </c>
+      <c r="C377" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D377" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F377" t="s">
+        <v>111</v>
+      </c>
+      <c r="K377" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A378" t="s">
+        <v>16</v>
+      </c>
+      <c r="B378" t="s">
+        <v>19</v>
+      </c>
+      <c r="C378" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D378" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F378" t="s">
+        <v>26</v>
+      </c>
+      <c r="K378" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A379" t="s">
+        <v>114</v>
+      </c>
+      <c r="B379" t="s">
+        <v>19</v>
+      </c>
+      <c r="C379" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D379" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F379" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A380" t="s">
+        <v>32</v>
+      </c>
+      <c r="B380" t="s">
+        <v>19</v>
+      </c>
+      <c r="C380" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D380" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F380" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A381" t="s">
+        <v>11</v>
+      </c>
+      <c r="B381" t="s">
+        <v>19</v>
+      </c>
+      <c r="C381" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D381" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F381" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A382" t="s">
+        <v>16</v>
+      </c>
+      <c r="B382" t="s">
+        <v>19</v>
+      </c>
+      <c r="C382" s="2">
+        <v>43816</v>
+      </c>
+      <c r="D382" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F382" t="s">
+        <v>26</v>
+      </c>
+      <c r="K382" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A383" t="s">
+        <v>17</v>
+      </c>
+      <c r="B383" t="s">
+        <v>19</v>
+      </c>
+      <c r="C383" s="2">
+        <v>43816</v>
+      </c>
+      <c r="D383" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F383" t="s">
+        <v>26</v>
+      </c>
+      <c r="K383" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated observations Completed April 2020, moving on to May
</commit_message>
<xml_diff>
--- a/data/auralObservations.xlsx
+++ b/data/auralObservations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\code\auralLandscapes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C386E6F6-BFD2-47DC-BEC2-2C38DAF3EC73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03689E-33D8-4656-B601-C1C667491E23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
+    <workbookView xWindow="0" yWindow="2115" windowWidth="10800" windowHeight="7830" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
   </bookViews>
   <sheets>
     <sheet name="observations" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="183">
   <si>
     <t>taxon</t>
   </si>
@@ -503,6 +503,81 @@
   </si>
   <si>
     <t>guessing at time -- morning walk w/ dog on a Saturday</t>
+  </si>
+  <si>
+    <t>guessing: evening after walk, but still light enough to see tree trunks. Pinning right around sunset</t>
+  </si>
+  <si>
+    <t>time and date only pinned: "A great horned owl has been calling in our neighborhood."</t>
+  </si>
+  <si>
+    <t>time estimated: morning walk b/f work, early in the pandemic</t>
+  </si>
+  <si>
+    <t>winter wren</t>
+  </si>
+  <si>
+    <t>time estimated: "this afternoon"</t>
+  </si>
+  <si>
+    <t>time estimated: morning walk, one of the first of the pandemic</t>
+  </si>
+  <si>
+    <t>time unspecified, but recorded in field notes as walk starting at 6:50</t>
+  </si>
+  <si>
+    <t>time unspecified: early morning, sitting downstairs reading, everyone quiet by 8:00.</t>
+  </si>
+  <si>
+    <t>sometime after 8, still a morning walk</t>
+  </si>
+  <si>
+    <t>brown creeper</t>
+  </si>
+  <si>
+    <t>hermit thrush</t>
+  </si>
+  <si>
+    <t>time unspecified, but likely to be observations on morning walk with brooklyn, after coffee with rachel</t>
+  </si>
+  <si>
+    <t>timestamp on iNaturalist photo</t>
+  </si>
+  <si>
+    <t>no time, but on morning walk with Rachel and Brooklyn, Sunday</t>
+  </si>
+  <si>
+    <t>"sun has just gone down"</t>
+  </si>
+  <si>
+    <t>timestamp on photo from that walk</t>
+  </si>
+  <si>
+    <t>reported as "what appeared to be a veery," but corrected to hermit thrush in later post</t>
+  </si>
+  <si>
+    <t>time estimated from a few photos on the walk</t>
+  </si>
+  <si>
+    <t>time from field notes</t>
+  </si>
+  <si>
+    <t>flicker</t>
+  </si>
+  <si>
+    <t>posted 4/3, but field notes are clear that this is the 4/2 walk; time from field notebook</t>
+  </si>
+  <si>
+    <t>downy woodpecker</t>
+  </si>
+  <si>
+    <t>Warrenville Rd, near intersection with 355</t>
+  </si>
+  <si>
+    <t>time inferred from train schedule cited in blog post; evening bike ride with David</t>
+  </si>
+  <si>
+    <t>time not specified,but morning, presumably b/f work</t>
   </si>
 </sst>
 </file>
@@ -890,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830C5A1-1504-4FB4-98E5-D787D6C4A5A6}">
-  <dimension ref="A1:K383"/>
+  <dimension ref="A1:K457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B364" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H382" sqref="H382"/>
+    <sheetView tabSelected="1" topLeftCell="A437" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A458" sqref="A458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9477,6 +9552,1405 @@
       </c>
       <c r="K383" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A384" t="s">
+        <v>11</v>
+      </c>
+      <c r="B384" t="s">
+        <v>19</v>
+      </c>
+      <c r="C384" s="2">
+        <v>43858</v>
+      </c>
+      <c r="D384" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F384" t="s">
+        <v>26</v>
+      </c>
+      <c r="K384" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A385" t="s">
+        <v>11</v>
+      </c>
+      <c r="B385" t="s">
+        <v>19</v>
+      </c>
+      <c r="C385" s="2">
+        <v>43875</v>
+      </c>
+      <c r="D385" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F385" t="s">
+        <v>111</v>
+      </c>
+      <c r="K385" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A386" t="s">
+        <v>10</v>
+      </c>
+      <c r="B386" t="s">
+        <v>19</v>
+      </c>
+      <c r="C386" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D386" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F386" t="s">
+        <v>26</v>
+      </c>
+      <c r="K386" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A387" t="s">
+        <v>7</v>
+      </c>
+      <c r="B387" t="s">
+        <v>19</v>
+      </c>
+      <c r="C387" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D387" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F387" t="s">
+        <v>26</v>
+      </c>
+      <c r="K387" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A388" t="s">
+        <v>17</v>
+      </c>
+      <c r="B388" t="s">
+        <v>19</v>
+      </c>
+      <c r="C388" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D388" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F388" t="s">
+        <v>26</v>
+      </c>
+      <c r="K388" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A389" t="s">
+        <v>154</v>
+      </c>
+      <c r="B389" t="s">
+        <v>19</v>
+      </c>
+      <c r="C389" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D389" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F389" t="s">
+        <v>26</v>
+      </c>
+      <c r="K389" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A390" t="s">
+        <v>16</v>
+      </c>
+      <c r="B390" t="s">
+        <v>19</v>
+      </c>
+      <c r="C390" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D390" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F390" t="s">
+        <v>26</v>
+      </c>
+      <c r="K390" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A391" t="s">
+        <v>87</v>
+      </c>
+      <c r="B391" t="s">
+        <v>19</v>
+      </c>
+      <c r="C391" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D391" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F391" t="s">
+        <v>26</v>
+      </c>
+      <c r="K391" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A392" t="s">
+        <v>161</v>
+      </c>
+      <c r="B392" t="s">
+        <v>19</v>
+      </c>
+      <c r="C392" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D392" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F392" t="s">
+        <v>26</v>
+      </c>
+      <c r="K392" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A393" t="s">
+        <v>32</v>
+      </c>
+      <c r="B393" t="s">
+        <v>19</v>
+      </c>
+      <c r="C393" s="2">
+        <v>43915</v>
+      </c>
+      <c r="D393" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F393" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A394" t="s">
+        <v>10</v>
+      </c>
+      <c r="B394" t="s">
+        <v>19</v>
+      </c>
+      <c r="C394" s="2">
+        <v>43914</v>
+      </c>
+      <c r="D394" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F394" t="s">
+        <v>40</v>
+      </c>
+      <c r="K394" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A395" t="s">
+        <v>62</v>
+      </c>
+      <c r="B395" t="s">
+        <v>19</v>
+      </c>
+      <c r="C395" s="2">
+        <v>43914</v>
+      </c>
+      <c r="D395" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F395" t="s">
+        <v>40</v>
+      </c>
+      <c r="K395" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A396" t="s">
+        <v>49</v>
+      </c>
+      <c r="B396" t="s">
+        <v>19</v>
+      </c>
+      <c r="C396" s="2">
+        <v>43914</v>
+      </c>
+      <c r="D396" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F396" t="s">
+        <v>40</v>
+      </c>
+      <c r="K396" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A397" t="s">
+        <v>16</v>
+      </c>
+      <c r="B397" t="s">
+        <v>19</v>
+      </c>
+      <c r="C397" s="2">
+        <v>43914</v>
+      </c>
+      <c r="D397" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F397" t="s">
+        <v>40</v>
+      </c>
+      <c r="K397" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A398" t="s">
+        <v>32</v>
+      </c>
+      <c r="B398" t="s">
+        <v>19</v>
+      </c>
+      <c r="C398" s="2">
+        <v>43913</v>
+      </c>
+      <c r="D398" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F398" t="s">
+        <v>26</v>
+      </c>
+      <c r="K398" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A399" t="s">
+        <v>16</v>
+      </c>
+      <c r="B399" t="s">
+        <v>19</v>
+      </c>
+      <c r="C399" s="2">
+        <v>43913</v>
+      </c>
+      <c r="D399" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F399" t="s">
+        <v>26</v>
+      </c>
+      <c r="K399" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A400" t="s">
+        <v>24</v>
+      </c>
+      <c r="B400" t="s">
+        <v>19</v>
+      </c>
+      <c r="C400" s="2">
+        <v>43913</v>
+      </c>
+      <c r="D400" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F400" t="s">
+        <v>26</v>
+      </c>
+      <c r="K400" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A401" t="s">
+        <v>52</v>
+      </c>
+      <c r="B401" t="s">
+        <v>19</v>
+      </c>
+      <c r="C401" s="2">
+        <v>43912</v>
+      </c>
+      <c r="D401" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F401" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A402" t="s">
+        <v>10</v>
+      </c>
+      <c r="B402" t="s">
+        <v>19</v>
+      </c>
+      <c r="C402" s="2">
+        <v>43912</v>
+      </c>
+      <c r="D402" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F402" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A403" t="s">
+        <v>32</v>
+      </c>
+      <c r="B403" t="s">
+        <v>19</v>
+      </c>
+      <c r="C403" s="2">
+        <v>43912</v>
+      </c>
+      <c r="D403" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F403" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A404" t="s">
+        <v>91</v>
+      </c>
+      <c r="B404" t="s">
+        <v>19</v>
+      </c>
+      <c r="C404" s="2">
+        <v>43912</v>
+      </c>
+      <c r="D404" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F404" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A405" t="s">
+        <v>101</v>
+      </c>
+      <c r="B405" t="s">
+        <v>19</v>
+      </c>
+      <c r="C405" s="2">
+        <v>43912</v>
+      </c>
+      <c r="D405" s="3">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F405" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A406" t="s">
+        <v>89</v>
+      </c>
+      <c r="B406" t="s">
+        <v>19</v>
+      </c>
+      <c r="C406" s="2">
+        <v>43949</v>
+      </c>
+      <c r="D406" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F406" t="s">
+        <v>26</v>
+      </c>
+      <c r="K406" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A407" t="s">
+        <v>71</v>
+      </c>
+      <c r="B407" t="s">
+        <v>19</v>
+      </c>
+      <c r="C407" s="2">
+        <v>43949</v>
+      </c>
+      <c r="D407" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F407" t="s">
+        <v>26</v>
+      </c>
+      <c r="K407" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A408" t="s">
+        <v>35</v>
+      </c>
+      <c r="B408" t="s">
+        <v>19</v>
+      </c>
+      <c r="C408" s="2">
+        <v>43949</v>
+      </c>
+      <c r="D408" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F408" t="s">
+        <v>26</v>
+      </c>
+      <c r="K408" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A409" t="s">
+        <v>161</v>
+      </c>
+      <c r="B409" t="s">
+        <v>19</v>
+      </c>
+      <c r="C409" s="2">
+        <v>43949</v>
+      </c>
+      <c r="D409" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F409" t="s">
+        <v>26</v>
+      </c>
+      <c r="K409" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A410" t="s">
+        <v>50</v>
+      </c>
+      <c r="B410" t="s">
+        <v>19</v>
+      </c>
+      <c r="C410" s="2">
+        <v>43949</v>
+      </c>
+      <c r="D410" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F410" t="s">
+        <v>26</v>
+      </c>
+      <c r="K410" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A411" t="s">
+        <v>7</v>
+      </c>
+      <c r="B411" t="s">
+        <v>19</v>
+      </c>
+      <c r="C411" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D411" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F411" t="s">
+        <v>111</v>
+      </c>
+      <c r="K411" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A412" t="s">
+        <v>35</v>
+      </c>
+      <c r="B412" t="s">
+        <v>19</v>
+      </c>
+      <c r="C412" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D412" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F412" t="s">
+        <v>111</v>
+      </c>
+      <c r="K412" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A413" t="s">
+        <v>58</v>
+      </c>
+      <c r="B413" t="s">
+        <v>47</v>
+      </c>
+      <c r="C413" s="2">
+        <v>43950</v>
+      </c>
+      <c r="D413" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="F413" t="s">
+        <v>111</v>
+      </c>
+      <c r="K413" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A414" t="s">
+        <v>167</v>
+      </c>
+      <c r="B414" t="s">
+        <v>19</v>
+      </c>
+      <c r="C414" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D414" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F414" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A415" t="s">
+        <v>32</v>
+      </c>
+      <c r="B415" t="s">
+        <v>19</v>
+      </c>
+      <c r="C415" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D415" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F415" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A416" t="s">
+        <v>34</v>
+      </c>
+      <c r="B416" t="s">
+        <v>19</v>
+      </c>
+      <c r="C416" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D416" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F416" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A417" t="s">
+        <v>7</v>
+      </c>
+      <c r="B417" t="s">
+        <v>19</v>
+      </c>
+      <c r="C417" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D417" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F417" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A418" t="s">
+        <v>52</v>
+      </c>
+      <c r="B418" t="s">
+        <v>19</v>
+      </c>
+      <c r="C418" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D418" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F418" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A419" t="s">
+        <v>17</v>
+      </c>
+      <c r="B419" t="s">
+        <v>19</v>
+      </c>
+      <c r="C419" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D419" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F419" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A420" t="s">
+        <v>62</v>
+      </c>
+      <c r="B420" t="s">
+        <v>19</v>
+      </c>
+      <c r="C420" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D420" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F420" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A421" t="s">
+        <v>168</v>
+      </c>
+      <c r="B421" t="s">
+        <v>19</v>
+      </c>
+      <c r="C421" s="2">
+        <v>43942</v>
+      </c>
+      <c r="D421" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F421" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A422" t="s">
+        <v>66</v>
+      </c>
+      <c r="B422" t="s">
+        <v>19</v>
+      </c>
+      <c r="C422" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D422" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F422" t="s">
+        <v>111</v>
+      </c>
+      <c r="K422" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A423" t="s">
+        <v>35</v>
+      </c>
+      <c r="B423" t="s">
+        <v>19</v>
+      </c>
+      <c r="C423" s="2">
+        <v>43945</v>
+      </c>
+      <c r="D423" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F423" t="s">
+        <v>111</v>
+      </c>
+      <c r="K423" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A424" t="s">
+        <v>167</v>
+      </c>
+      <c r="B424" t="s">
+        <v>19</v>
+      </c>
+      <c r="C424" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D424" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F424" t="s">
+        <v>26</v>
+      </c>
+      <c r="K424" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A425" t="s">
+        <v>34</v>
+      </c>
+      <c r="B425" t="s">
+        <v>19</v>
+      </c>
+      <c r="C425" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D425" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F425" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A426" t="s">
+        <v>7</v>
+      </c>
+      <c r="B426" t="s">
+        <v>19</v>
+      </c>
+      <c r="C426" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D426" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F426" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A427" t="s">
+        <v>10</v>
+      </c>
+      <c r="B427" t="s">
+        <v>19</v>
+      </c>
+      <c r="C427" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D427" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F427" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A428" t="s">
+        <v>16</v>
+      </c>
+      <c r="B428" t="s">
+        <v>19</v>
+      </c>
+      <c r="C428" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D428" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F428" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A429" t="s">
+        <v>32</v>
+      </c>
+      <c r="B429" t="s">
+        <v>19</v>
+      </c>
+      <c r="C429" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D429" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F429" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A430" t="s">
+        <v>86</v>
+      </c>
+      <c r="B430" t="s">
+        <v>19</v>
+      </c>
+      <c r="C430" s="2">
+        <v>43939</v>
+      </c>
+      <c r="D430" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F430" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A431" t="s">
+        <v>34</v>
+      </c>
+      <c r="B431" t="s">
+        <v>19</v>
+      </c>
+      <c r="C431" s="2">
+        <v>43940</v>
+      </c>
+      <c r="D431" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F431" t="s">
+        <v>26</v>
+      </c>
+      <c r="K431" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A432" t="s">
+        <v>52</v>
+      </c>
+      <c r="B432" t="s">
+        <v>19</v>
+      </c>
+      <c r="C432" s="2">
+        <v>43940</v>
+      </c>
+      <c r="D432" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F432" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A433" t="s">
+        <v>32</v>
+      </c>
+      <c r="B433" t="s">
+        <v>19</v>
+      </c>
+      <c r="C433" s="2">
+        <v>43940</v>
+      </c>
+      <c r="D433" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F433" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A434" t="s">
+        <v>50</v>
+      </c>
+      <c r="B434" t="s">
+        <v>19</v>
+      </c>
+      <c r="C434" s="2">
+        <v>43940</v>
+      </c>
+      <c r="D434" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F434" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A435" t="s">
+        <v>86</v>
+      </c>
+      <c r="B435" t="s">
+        <v>19</v>
+      </c>
+      <c r="C435" s="2">
+        <v>43940</v>
+      </c>
+      <c r="D435" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F435" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A436" t="s">
+        <v>7</v>
+      </c>
+      <c r="B436" t="s">
+        <v>19</v>
+      </c>
+      <c r="C436" s="2">
+        <v>43940</v>
+      </c>
+      <c r="D436" s="3">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="F436" t="s">
+        <v>111</v>
+      </c>
+      <c r="K436" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A437" t="s">
+        <v>52</v>
+      </c>
+      <c r="B437" t="s">
+        <v>19</v>
+      </c>
+      <c r="C437" s="2">
+        <v>43935</v>
+      </c>
+      <c r="D437" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F437" t="s">
+        <v>26</v>
+      </c>
+      <c r="K437" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A438" t="s">
+        <v>7</v>
+      </c>
+      <c r="B438" t="s">
+        <v>19</v>
+      </c>
+      <c r="C438" s="2">
+        <v>43935</v>
+      </c>
+      <c r="D438" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F438" t="s">
+        <v>26</v>
+      </c>
+      <c r="K438" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="439" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A439" t="s">
+        <v>168</v>
+      </c>
+      <c r="B439" t="s">
+        <v>19</v>
+      </c>
+      <c r="C439" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D439" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F439" t="s">
+        <v>26</v>
+      </c>
+      <c r="K439" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="440" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A440" t="s">
+        <v>86</v>
+      </c>
+      <c r="B440" t="s">
+        <v>19</v>
+      </c>
+      <c r="C440" s="2">
+        <v>43936</v>
+      </c>
+      <c r="D440" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F440" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A441" t="s">
+        <v>161</v>
+      </c>
+      <c r="B441" t="s">
+        <v>19</v>
+      </c>
+      <c r="C441" s="2">
+        <v>43930</v>
+      </c>
+      <c r="D441" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F441" t="s">
+        <v>26</v>
+      </c>
+      <c r="K441" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="442" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A442" t="s">
+        <v>50</v>
+      </c>
+      <c r="B442" t="s">
+        <v>47</v>
+      </c>
+      <c r="C442" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D442" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F442" t="s">
+        <v>26</v>
+      </c>
+      <c r="K442" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="443" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A443" t="s">
+        <v>49</v>
+      </c>
+      <c r="B443" t="s">
+        <v>47</v>
+      </c>
+      <c r="C443" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D443" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F443" t="s">
+        <v>26</v>
+      </c>
+      <c r="K443" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A444" t="s">
+        <v>177</v>
+      </c>
+      <c r="B444" t="s">
+        <v>47</v>
+      </c>
+      <c r="C444" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D444" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F444" t="s">
+        <v>26</v>
+      </c>
+      <c r="K444" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="445" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A445" t="s">
+        <v>32</v>
+      </c>
+      <c r="B445" t="s">
+        <v>47</v>
+      </c>
+      <c r="C445" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D445" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F445" t="s">
+        <v>26</v>
+      </c>
+      <c r="K445" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="446" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A446" t="s">
+        <v>10</v>
+      </c>
+      <c r="B446" t="s">
+        <v>47</v>
+      </c>
+      <c r="C446" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D446" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F446" t="s">
+        <v>26</v>
+      </c>
+      <c r="K446" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="447" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A447" t="s">
+        <v>7</v>
+      </c>
+      <c r="B447" t="s">
+        <v>47</v>
+      </c>
+      <c r="C447" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D447" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F447" t="s">
+        <v>26</v>
+      </c>
+      <c r="K447" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="448" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A448" t="s">
+        <v>52</v>
+      </c>
+      <c r="B448" t="s">
+        <v>47</v>
+      </c>
+      <c r="C448" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D448" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F448" t="s">
+        <v>26</v>
+      </c>
+      <c r="K448" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="449" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A449" t="s">
+        <v>56</v>
+      </c>
+      <c r="B449" t="s">
+        <v>47</v>
+      </c>
+      <c r="C449" s="2">
+        <v>43929</v>
+      </c>
+      <c r="D449" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F449" t="s">
+        <v>26</v>
+      </c>
+      <c r="K449" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="450" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A450" t="s">
+        <v>87</v>
+      </c>
+      <c r="B450" t="s">
+        <v>19</v>
+      </c>
+      <c r="C450" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D450" s="3">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F450" t="s">
+        <v>26</v>
+      </c>
+      <c r="K450" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="451" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A451" t="s">
+        <v>32</v>
+      </c>
+      <c r="B451" t="s">
+        <v>19</v>
+      </c>
+      <c r="C451" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D451" s="3">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F451" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="452" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A452" t="s">
+        <v>179</v>
+      </c>
+      <c r="B452" t="s">
+        <v>19</v>
+      </c>
+      <c r="C452" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D452" s="3">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F452" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="453" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A453" t="s">
+        <v>32</v>
+      </c>
+      <c r="B453" t="s">
+        <v>19</v>
+      </c>
+      <c r="C453" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D453" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F453" t="s">
+        <v>26</v>
+      </c>
+      <c r="K453" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="454" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A454" t="s">
+        <v>62</v>
+      </c>
+      <c r="B454" t="s">
+        <v>19</v>
+      </c>
+      <c r="C454" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D454" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F454" t="s">
+        <v>180</v>
+      </c>
+      <c r="K454" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="455" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A455" t="s">
+        <v>49</v>
+      </c>
+      <c r="B455" t="s">
+        <v>19</v>
+      </c>
+      <c r="C455" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D455" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F455" t="s">
+        <v>180</v>
+      </c>
+      <c r="K455" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="456" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A456" t="s">
+        <v>33</v>
+      </c>
+      <c r="B456" t="s">
+        <v>19</v>
+      </c>
+      <c r="C456" s="2">
+        <v>43923</v>
+      </c>
+      <c r="D456" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F456" t="s">
+        <v>180</v>
+      </c>
+      <c r="K456" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="457" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A457" t="s">
+        <v>167</v>
+      </c>
+      <c r="B457" t="s">
+        <v>19</v>
+      </c>
+      <c r="C457" s="2">
+        <v>43920</v>
+      </c>
+      <c r="D457" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F457" t="s">
+        <v>111</v>
+      </c>
+      <c r="K457" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating observations through May 2020
</commit_message>
<xml_diff>
--- a/data/auralObservations.xlsx
+++ b/data/auralObservations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\code\auralLandscapes\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahipp\Documents\CODE\auralLandscapes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03689E-33D8-4656-B601-C1C667491E23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42CCDDF-B82C-473A-BA64-AC8E9D5BEFBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2115" windowWidth="10800" windowHeight="7830" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="194">
   <si>
     <t>taxon</t>
   </si>
@@ -578,6 +578,39 @@
   </si>
   <si>
     <t>time not specified,but morning, presumably b/f work</t>
+  </si>
+  <si>
+    <t>time unspecified; morning dog walk</t>
+  </si>
+  <si>
+    <t>chestnut-sided warbler</t>
+  </si>
+  <si>
+    <t>10 a.m. placeholder for daylong observations</t>
+  </si>
+  <si>
+    <t>timestamp on white-breasted nuthatch photo</t>
+  </si>
+  <si>
+    <t>at the end of the day; no time specified</t>
+  </si>
+  <si>
+    <t>time from field notebook</t>
+  </si>
+  <si>
+    <t>… assumed later, as this was observed on the alk out</t>
+  </si>
+  <si>
+    <t>time from photo timestamp</t>
+  </si>
+  <si>
+    <t>northern parula</t>
+  </si>
+  <si>
+    <t>timestamp on white bear sedge photo observed at same time</t>
+  </si>
+  <si>
+    <t>chimney swift</t>
   </si>
 </sst>
 </file>
@@ -965,27 +998,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830C5A1-1504-4FB4-98E5-D787D6C4A5A6}">
-  <dimension ref="A1:K457"/>
+  <dimension ref="A1:K488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A437" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A458" sqref="A458"/>
+    <sheetView tabSelected="1" topLeftCell="A456" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C485" sqref="C485"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.40625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.40625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.86328125" customWidth="1"/>
-    <col min="8" max="8" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1053,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1066,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1089,7 +1122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1112,7 +1145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1204,7 +1237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1227,7 +1260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +1283,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1319,7 +1352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1342,7 +1375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1365,7 +1398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1388,7 +1421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1444,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1467,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1457,7 +1490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1548,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1541,7 +1574,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1593,7 +1626,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1619,7 +1652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1645,7 +1678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1668,7 +1701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1691,7 +1724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1714,7 +1747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1737,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1760,7 +1793,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1783,7 +1816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1806,7 +1839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1832,7 +1865,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1858,7 +1891,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1884,7 +1917,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1910,7 +1943,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1936,7 +1969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -1962,7 +1995,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1988,7 +2021,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -2014,7 +2047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2040,7 +2073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -2066,7 +2099,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2092,7 +2125,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -2118,7 +2151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -2144,7 +2177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2170,7 +2203,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2196,7 +2229,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2222,7 +2255,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -2248,7 +2281,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -2274,7 +2307,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2300,7 +2333,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2326,7 +2359,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -2349,7 +2382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -2372,7 +2405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>33</v>
       </c>
@@ -2395,7 +2428,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -2418,7 +2451,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2441,7 +2474,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>52</v>
       </c>
@@ -2464,7 +2497,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>35</v>
       </c>
@@ -2487,7 +2520,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2510,7 +2543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -2536,7 +2569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -2562,7 +2595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -2588,7 +2621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -2614,7 +2647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -2640,7 +2673,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>33</v>
       </c>
@@ -2666,7 +2699,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -2692,7 +2725,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>62</v>
       </c>
@@ -2718,7 +2751,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>58</v>
       </c>
@@ -2744,7 +2777,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -2770,7 +2803,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2796,7 +2829,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -2822,7 +2855,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>50</v>
       </c>
@@ -2848,7 +2881,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>49</v>
       </c>
@@ -2874,7 +2907,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>59</v>
       </c>
@@ -2900,7 +2933,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>66</v>
       </c>
@@ -2926,7 +2959,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -2952,7 +2985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>50</v>
       </c>
@@ -2978,7 +3011,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>71</v>
       </c>
@@ -3004,7 +3037,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>72</v>
       </c>
@@ -3030,7 +3063,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -3056,7 +3089,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -3082,7 +3115,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>73</v>
       </c>
@@ -3108,7 +3141,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -3134,7 +3167,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>32</v>
       </c>
@@ -3160,7 +3193,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
@@ -3186,7 +3219,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -3209,7 +3242,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>66</v>
       </c>
@@ -3232,7 +3265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -3255,7 +3288,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>78</v>
       </c>
@@ -3278,7 +3311,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>79</v>
       </c>
@@ -3301,7 +3334,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -3324,7 +3357,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>62</v>
       </c>
@@ -3350,7 +3383,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>73</v>
       </c>
@@ -3376,7 +3409,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>36</v>
       </c>
@@ -3402,7 +3435,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -3428,7 +3461,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>59</v>
       </c>
@@ -3454,7 +3487,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>66</v>
       </c>
@@ -3480,7 +3513,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>60</v>
       </c>
@@ -3506,7 +3539,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>72</v>
       </c>
@@ -3532,7 +3565,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>83</v>
       </c>
@@ -3558,7 +3591,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>75</v>
       </c>
@@ -3584,7 +3617,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>84</v>
       </c>
@@ -3610,7 +3643,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -3636,7 +3669,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>52</v>
       </c>
@@ -3662,7 +3695,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>85</v>
       </c>
@@ -3688,7 +3721,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>86</v>
       </c>
@@ -3714,7 +3747,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>78</v>
       </c>
@@ -3740,7 +3773,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>62</v>
       </c>
@@ -3766,7 +3799,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -3792,7 +3825,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -3818,7 +3851,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>73</v>
       </c>
@@ -3844,7 +3877,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>60</v>
       </c>
@@ -3870,7 +3903,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>66</v>
       </c>
@@ -3896,7 +3929,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>12</v>
       </c>
@@ -3922,7 +3955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>49</v>
       </c>
@@ -3948,7 +3981,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>59</v>
       </c>
@@ -3974,7 +4007,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>52</v>
       </c>
@@ -4000,7 +4033,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>83</v>
       </c>
@@ -4026,7 +4059,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>87</v>
       </c>
@@ -4052,7 +4085,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -4078,7 +4111,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>84</v>
       </c>
@@ -4104,7 +4137,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>73</v>
       </c>
@@ -4130,7 +4163,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>62</v>
       </c>
@@ -4156,7 +4189,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>89</v>
       </c>
@@ -4182,7 +4215,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>12</v>
       </c>
@@ -4208,7 +4241,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>10</v>
       </c>
@@ -4231,7 +4264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>62</v>
       </c>
@@ -4257,7 +4290,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -4283,7 +4316,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>12</v>
       </c>
@@ -4309,7 +4342,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>35</v>
       </c>
@@ -4335,7 +4368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -4361,7 +4394,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>90</v>
       </c>
@@ -4387,7 +4420,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>91</v>
       </c>
@@ -4413,7 +4446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -4439,7 +4472,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>33</v>
       </c>
@@ -4465,7 +4498,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>35</v>
       </c>
@@ -4491,7 +4524,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>36</v>
       </c>
@@ -4517,7 +4550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>56</v>
       </c>
@@ -4543,7 +4576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>89</v>
       </c>
@@ -4569,7 +4602,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>72</v>
       </c>
@@ -4592,7 +4625,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>92</v>
       </c>
@@ -4615,7 +4648,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>12</v>
       </c>
@@ -4638,7 +4671,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>36</v>
       </c>
@@ -4664,7 +4697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>94</v>
       </c>
@@ -4690,7 +4723,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>49</v>
       </c>
@@ -4713,7 +4746,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>96</v>
       </c>
@@ -4736,7 +4769,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>35</v>
       </c>
@@ -4759,7 +4792,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>33</v>
       </c>
@@ -4782,7 +4815,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -4805,7 +4838,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>97</v>
       </c>
@@ -4828,7 +4861,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>16</v>
       </c>
@@ -4851,7 +4884,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>32</v>
       </c>
@@ -4874,7 +4907,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>52</v>
       </c>
@@ -4897,7 +4930,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>17</v>
       </c>
@@ -4920,7 +4953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>98</v>
       </c>
@@ -4943,7 +4976,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>33</v>
       </c>
@@ -4966,7 +4999,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>13</v>
       </c>
@@ -4989,7 +5022,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>60</v>
       </c>
@@ -5012,7 +5045,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>99</v>
       </c>
@@ -5035,7 +5068,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>51</v>
       </c>
@@ -5055,7 +5088,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>10</v>
       </c>
@@ -5075,7 +5108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>60</v>
       </c>
@@ -5095,7 +5128,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>49</v>
       </c>
@@ -5115,7 +5148,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>52</v>
       </c>
@@ -5135,7 +5168,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>16</v>
       </c>
@@ -5155,7 +5188,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>7</v>
       </c>
@@ -5175,7 +5208,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>10</v>
       </c>
@@ -5195,7 +5228,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>24</v>
       </c>
@@ -5215,7 +5248,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>7</v>
       </c>
@@ -5235,7 +5268,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>10</v>
       </c>
@@ -5255,7 +5288,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -5275,7 +5308,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>32</v>
       </c>
@@ -5295,7 +5328,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>101</v>
       </c>
@@ -5318,7 +5351,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>7</v>
       </c>
@@ -5338,7 +5371,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>51</v>
       </c>
@@ -5358,7 +5391,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>33</v>
       </c>
@@ -5378,7 +5411,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>62</v>
       </c>
@@ -5398,7 +5431,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>32</v>
       </c>
@@ -5418,7 +5451,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>52</v>
       </c>
@@ -5438,7 +5471,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>10</v>
       </c>
@@ -5458,7 +5491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>7</v>
       </c>
@@ -5478,7 +5511,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>83</v>
       </c>
@@ -5498,7 +5531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>66</v>
       </c>
@@ -5518,7 +5551,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>62</v>
       </c>
@@ -5538,7 +5571,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>33</v>
       </c>
@@ -5558,7 +5591,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>52</v>
       </c>
@@ -5578,7 +5611,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>10</v>
       </c>
@@ -5598,7 +5631,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -5618,7 +5651,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>24</v>
       </c>
@@ -5638,7 +5671,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -5658,7 +5691,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>7</v>
       </c>
@@ -5678,7 +5711,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>10</v>
       </c>
@@ -5698,7 +5731,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>33</v>
       </c>
@@ -5721,7 +5754,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>62</v>
       </c>
@@ -5744,7 +5777,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>49</v>
       </c>
@@ -5767,7 +5800,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>56</v>
       </c>
@@ -5790,7 +5823,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>60</v>
       </c>
@@ -5813,7 +5846,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>50</v>
       </c>
@@ -5836,7 +5869,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>52</v>
       </c>
@@ -5859,7 +5892,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -5882,7 +5915,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>86</v>
       </c>
@@ -5905,7 +5938,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>72</v>
       </c>
@@ -5928,7 +5961,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>92</v>
       </c>
@@ -5951,7 +5984,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>59</v>
       </c>
@@ -5974,7 +6007,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>33</v>
       </c>
@@ -5997,7 +6030,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>66</v>
       </c>
@@ -6020,7 +6053,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>36</v>
       </c>
@@ -6043,7 +6076,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>84</v>
       </c>
@@ -6066,7 +6099,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>105</v>
       </c>
@@ -6089,7 +6122,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>72</v>
       </c>
@@ -6112,7 +6145,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>62</v>
       </c>
@@ -6135,7 +6168,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>17</v>
       </c>
@@ -6158,7 +6191,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>58</v>
       </c>
@@ -6181,7 +6214,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>36</v>
       </c>
@@ -6204,7 +6237,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>75</v>
       </c>
@@ -6227,7 +6260,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>35</v>
       </c>
@@ -6250,7 +6283,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>66</v>
       </c>
@@ -6273,7 +6306,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>91</v>
       </c>
@@ -6296,7 +6329,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>75</v>
       </c>
@@ -6319,7 +6352,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>84</v>
       </c>
@@ -6342,7 +6375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>60</v>
       </c>
@@ -6365,7 +6398,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>32</v>
       </c>
@@ -6388,7 +6421,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>79</v>
       </c>
@@ -6411,7 +6444,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>35</v>
       </c>
@@ -6434,7 +6467,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>87</v>
       </c>
@@ -6457,7 +6490,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>33</v>
       </c>
@@ -6480,7 +6513,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>59</v>
       </c>
@@ -6503,7 +6536,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>13</v>
       </c>
@@ -6526,7 +6559,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>109</v>
       </c>
@@ -6549,7 +6582,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>83</v>
       </c>
@@ -6572,7 +6605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>34</v>
       </c>
@@ -6595,7 +6628,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>73</v>
       </c>
@@ -6618,7 +6651,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>84</v>
       </c>
@@ -6641,7 +6674,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>92</v>
       </c>
@@ -6664,7 +6697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>110</v>
       </c>
@@ -6687,7 +6720,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>89</v>
       </c>
@@ -6710,7 +6743,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>71</v>
       </c>
@@ -6733,7 +6766,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>72</v>
       </c>
@@ -6753,7 +6786,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>72</v>
       </c>
@@ -6773,7 +6806,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>7</v>
       </c>
@@ -6793,7 +6826,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>32</v>
       </c>
@@ -6813,7 +6846,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>75</v>
       </c>
@@ -6833,7 +6866,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>71</v>
       </c>
@@ -6853,7 +6886,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>58</v>
       </c>
@@ -6873,7 +6906,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>58</v>
       </c>
@@ -6896,7 +6929,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>7</v>
       </c>
@@ -6916,7 +6949,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>71</v>
       </c>
@@ -6936,7 +6969,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>13</v>
       </c>
@@ -6956,7 +6989,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>94</v>
       </c>
@@ -6976,7 +7009,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>21</v>
       </c>
@@ -6996,7 +7029,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>10</v>
       </c>
@@ -7016,7 +7049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>71</v>
       </c>
@@ -7039,7 +7072,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>10</v>
       </c>
@@ -7059,7 +7092,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>94</v>
       </c>
@@ -7079,7 +7112,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>10</v>
       </c>
@@ -7099,7 +7132,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>10</v>
       </c>
@@ -7119,7 +7152,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>10</v>
       </c>
@@ -7139,7 +7172,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>72</v>
       </c>
@@ -7159,7 +7192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>96</v>
       </c>
@@ -7179,7 +7212,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>73</v>
       </c>
@@ -7199,7 +7232,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>59</v>
       </c>
@@ -7219,7 +7252,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>66</v>
       </c>
@@ -7239,7 +7272,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>92</v>
       </c>
@@ -7259,7 +7292,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>7</v>
       </c>
@@ -7279,7 +7312,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>60</v>
       </c>
@@ -7299,7 +7332,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>92</v>
       </c>
@@ -7319,7 +7352,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>72</v>
       </c>
@@ -7339,7 +7372,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>91</v>
       </c>
@@ -7359,7 +7392,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>52</v>
       </c>
@@ -7379,7 +7412,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>84</v>
       </c>
@@ -7399,7 +7432,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>96</v>
       </c>
@@ -7419,7 +7452,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>11</v>
       </c>
@@ -7439,7 +7472,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>94</v>
       </c>
@@ -7459,7 +7492,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>39</v>
       </c>
@@ -7479,7 +7512,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>10</v>
       </c>
@@ -7499,7 +7532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>113</v>
       </c>
@@ -7522,7 +7555,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>16</v>
       </c>
@@ -7542,7 +7575,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>114</v>
       </c>
@@ -7562,7 +7595,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>10</v>
       </c>
@@ -7582,7 +7615,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>10</v>
       </c>
@@ -7602,7 +7635,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>16</v>
       </c>
@@ -7622,7 +7655,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>10</v>
       </c>
@@ -7642,7 +7675,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>17</v>
       </c>
@@ -7665,7 +7698,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>32</v>
       </c>
@@ -7688,7 +7721,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>50</v>
       </c>
@@ -7711,7 +7744,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>87</v>
       </c>
@@ -7734,7 +7767,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>13</v>
       </c>
@@ -7754,7 +7787,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>59</v>
       </c>
@@ -7774,7 +7807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>7</v>
       </c>
@@ -7794,7 +7827,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>33</v>
       </c>
@@ -7814,7 +7847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>60</v>
       </c>
@@ -7834,7 +7867,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>86</v>
       </c>
@@ -7854,7 +7887,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>58</v>
       </c>
@@ -7877,7 +7910,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>49</v>
       </c>
@@ -7900,7 +7933,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>50</v>
       </c>
@@ -7923,7 +7956,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>58</v>
       </c>
@@ -7946,7 +7979,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>122</v>
       </c>
@@ -7969,7 +8002,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>87</v>
       </c>
@@ -7992,7 +8025,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>33</v>
       </c>
@@ -8015,7 +8048,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>35</v>
       </c>
@@ -8035,7 +8068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>50</v>
       </c>
@@ -8058,7 +8091,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>49</v>
       </c>
@@ -8078,7 +8111,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>49</v>
       </c>
@@ -8101,7 +8134,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>52</v>
       </c>
@@ -8121,7 +8154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>7</v>
       </c>
@@ -8141,7 +8174,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>127</v>
       </c>
@@ -8161,7 +8194,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>72</v>
       </c>
@@ -8181,7 +8214,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>58</v>
       </c>
@@ -8201,7 +8234,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>50</v>
       </c>
@@ -8221,7 +8254,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>72</v>
       </c>
@@ -8241,7 +8274,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>92</v>
       </c>
@@ -8258,7 +8291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>84</v>
       </c>
@@ -8275,7 +8308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>75</v>
       </c>
@@ -8292,7 +8325,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>130</v>
       </c>
@@ -8309,7 +8342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>105</v>
       </c>
@@ -8326,7 +8359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>73</v>
       </c>
@@ -8343,7 +8376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>105</v>
       </c>
@@ -8360,7 +8393,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>89</v>
       </c>
@@ -8377,7 +8410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>88</v>
       </c>
@@ -8394,7 +8427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>79</v>
       </c>
@@ -8414,7 +8447,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>126</v>
       </c>
@@ -8434,7 +8467,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>85</v>
       </c>
@@ -8454,7 +8487,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>36</v>
       </c>
@@ -8474,7 +8507,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>58</v>
       </c>
@@ -8494,7 +8527,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>58</v>
       </c>
@@ -8514,7 +8547,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>94</v>
       </c>
@@ -8534,7 +8567,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>92</v>
       </c>
@@ -8554,7 +8587,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>109</v>
       </c>
@@ -8574,7 +8607,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>75</v>
       </c>
@@ -8594,7 +8627,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>126</v>
       </c>
@@ -8611,7 +8644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>75</v>
       </c>
@@ -8631,7 +8664,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>36</v>
       </c>
@@ -8651,7 +8684,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>7</v>
       </c>
@@ -8668,7 +8701,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>10</v>
       </c>
@@ -8688,7 +8721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>11</v>
       </c>
@@ -8708,7 +8741,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>58</v>
       </c>
@@ -8728,7 +8761,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>71</v>
       </c>
@@ -8748,7 +8781,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>84</v>
       </c>
@@ -8768,7 +8801,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>72</v>
       </c>
@@ -8788,7 +8821,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>32</v>
       </c>
@@ -8808,7 +8841,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>75</v>
       </c>
@@ -8828,7 +8861,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>75</v>
       </c>
@@ -8848,7 +8881,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>72</v>
       </c>
@@ -8868,7 +8901,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>71</v>
       </c>
@@ -8888,7 +8921,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>11</v>
       </c>
@@ -8908,7 +8941,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>143</v>
       </c>
@@ -8928,7 +8961,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>72</v>
       </c>
@@ -8948,7 +8981,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>92</v>
       </c>
@@ -8968,7 +9001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>7</v>
       </c>
@@ -8988,7 +9021,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>12</v>
       </c>
@@ -9008,7 +9041,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>71</v>
       </c>
@@ -9028,7 +9061,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>16</v>
       </c>
@@ -9048,7 +9081,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>59</v>
       </c>
@@ -9068,7 +9101,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>16</v>
       </c>
@@ -9085,7 +9118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>72</v>
       </c>
@@ -9102,7 +9135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>146</v>
       </c>
@@ -9119,7 +9152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>143</v>
       </c>
@@ -9136,7 +9169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>72</v>
       </c>
@@ -9153,7 +9186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>146</v>
       </c>
@@ -9170,7 +9203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>87</v>
       </c>
@@ -9187,7 +9220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>33</v>
       </c>
@@ -9204,7 +9237,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>72</v>
       </c>
@@ -9224,7 +9257,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>146</v>
       </c>
@@ -9244,7 +9277,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>21</v>
       </c>
@@ -9264,7 +9297,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>51</v>
       </c>
@@ -9284,7 +9317,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>146</v>
       </c>
@@ -9301,7 +9334,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>50</v>
       </c>
@@ -9321,7 +9354,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>50</v>
       </c>
@@ -9338,7 +9371,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>50</v>
       </c>
@@ -9355,7 +9388,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>51</v>
       </c>
@@ -9372,7 +9405,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>154</v>
       </c>
@@ -9389,7 +9422,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>7</v>
       </c>
@@ -9406,7 +9439,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>11</v>
       </c>
@@ -9423,7 +9456,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>101</v>
       </c>
@@ -9443,7 +9476,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>16</v>
       </c>
@@ -9463,7 +9496,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>114</v>
       </c>
@@ -9480,7 +9513,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>32</v>
       </c>
@@ -9497,7 +9530,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>11</v>
       </c>
@@ -9514,7 +9547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>16</v>
       </c>
@@ -9534,7 +9567,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>17</v>
       </c>
@@ -9554,7 +9587,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>11</v>
       </c>
@@ -9574,7 +9607,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>11</v>
       </c>
@@ -9594,7 +9627,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>10</v>
       </c>
@@ -9614,7 +9647,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>7</v>
       </c>
@@ -9634,7 +9667,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>17</v>
       </c>
@@ -9654,7 +9687,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>154</v>
       </c>
@@ -9674,7 +9707,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>16</v>
       </c>
@@ -9694,7 +9727,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>87</v>
       </c>
@@ -9714,7 +9747,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>161</v>
       </c>
@@ -9734,7 +9767,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>32</v>
       </c>
@@ -9751,7 +9784,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>10</v>
       </c>
@@ -9771,7 +9804,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>62</v>
       </c>
@@ -9791,7 +9824,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>49</v>
       </c>
@@ -9811,7 +9844,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>16</v>
       </c>
@@ -9831,7 +9864,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>32</v>
       </c>
@@ -9851,7 +9884,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>16</v>
       </c>
@@ -9871,7 +9904,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>24</v>
       </c>
@@ -9891,7 +9924,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>52</v>
       </c>
@@ -9908,7 +9941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>10</v>
       </c>
@@ -9925,7 +9958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>32</v>
       </c>
@@ -9942,7 +9975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>91</v>
       </c>
@@ -9959,7 +9992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>101</v>
       </c>
@@ -9976,7 +10009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>89</v>
       </c>
@@ -9996,7 +10029,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>71</v>
       </c>
@@ -10016,7 +10049,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>35</v>
       </c>
@@ -10036,7 +10069,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>161</v>
       </c>
@@ -10056,7 +10089,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>50</v>
       </c>
@@ -10076,7 +10109,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>7</v>
       </c>
@@ -10096,7 +10129,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>35</v>
       </c>
@@ -10116,7 +10149,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>58</v>
       </c>
@@ -10136,7 +10169,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>167</v>
       </c>
@@ -10153,7 +10186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>32</v>
       </c>
@@ -10170,7 +10203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>34</v>
       </c>
@@ -10187,7 +10220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>7</v>
       </c>
@@ -10204,7 +10237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>52</v>
       </c>
@@ -10221,7 +10254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>17</v>
       </c>
@@ -10238,7 +10271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>62</v>
       </c>
@@ -10255,7 +10288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>168</v>
       </c>
@@ -10272,7 +10305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>66</v>
       </c>
@@ -10292,7 +10325,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>35</v>
       </c>
@@ -10312,7 +10345,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>167</v>
       </c>
@@ -10332,7 +10365,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>34</v>
       </c>
@@ -10349,7 +10382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>7</v>
       </c>
@@ -10366,7 +10399,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>10</v>
       </c>
@@ -10383,7 +10416,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>16</v>
       </c>
@@ -10400,7 +10433,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>32</v>
       </c>
@@ -10417,7 +10450,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>86</v>
       </c>
@@ -10434,7 +10467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>34</v>
       </c>
@@ -10454,7 +10487,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>52</v>
       </c>
@@ -10471,7 +10504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="433" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>32</v>
       </c>
@@ -10488,7 +10521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>50</v>
       </c>
@@ -10505,7 +10538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>86</v>
       </c>
@@ -10522,7 +10555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>7</v>
       </c>
@@ -10542,7 +10575,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>52</v>
       </c>
@@ -10562,7 +10595,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>7</v>
       </c>
@@ -10582,7 +10615,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>168</v>
       </c>
@@ -10602,7 +10635,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="440" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>86</v>
       </c>
@@ -10619,7 +10652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>161</v>
       </c>
@@ -10639,7 +10672,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="442" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>50</v>
       </c>
@@ -10659,7 +10692,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="443" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>49</v>
       </c>
@@ -10679,7 +10712,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="444" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>177</v>
       </c>
@@ -10699,7 +10732,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="445" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>32</v>
       </c>
@@ -10719,7 +10752,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="446" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>10</v>
       </c>
@@ -10739,7 +10772,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="447" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>7</v>
       </c>
@@ -10759,7 +10792,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="448" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>52</v>
       </c>
@@ -10779,7 +10812,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>56</v>
       </c>
@@ -10799,7 +10832,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>87</v>
       </c>
@@ -10819,7 +10852,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>32</v>
       </c>
@@ -10836,7 +10869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>179</v>
       </c>
@@ -10853,7 +10886,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>32</v>
       </c>
@@ -10873,7 +10906,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>62</v>
       </c>
@@ -10893,7 +10926,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>49</v>
       </c>
@@ -10913,7 +10946,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>33</v>
       </c>
@@ -10933,7 +10966,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>167</v>
       </c>
@@ -10953,9 +10986,608 @@
         <v>182</v>
       </c>
     </row>
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>184</v>
+      </c>
+      <c r="B458" t="s">
+        <v>19</v>
+      </c>
+      <c r="C458" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D458" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F458" t="s">
+        <v>111</v>
+      </c>
+      <c r="K458" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>105</v>
+      </c>
+      <c r="B459" t="s">
+        <v>19</v>
+      </c>
+      <c r="C459" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D459" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F459" t="s">
+        <v>111</v>
+      </c>
+      <c r="K459" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>72</v>
+      </c>
+      <c r="B460" t="s">
+        <v>19</v>
+      </c>
+      <c r="C460" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D460" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F460" t="s">
+        <v>111</v>
+      </c>
+      <c r="K460" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="461" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>58</v>
+      </c>
+      <c r="B461" t="s">
+        <v>47</v>
+      </c>
+      <c r="C461" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D461" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F461" t="s">
+        <v>111</v>
+      </c>
+      <c r="K461" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>36</v>
+      </c>
+      <c r="B462" t="s">
+        <v>19</v>
+      </c>
+      <c r="C462" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D462" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F462" t="s">
+        <v>40</v>
+      </c>
+      <c r="K462" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>85</v>
+      </c>
+      <c r="B463" t="s">
+        <v>19</v>
+      </c>
+      <c r="C463" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D463" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F463" t="s">
+        <v>40</v>
+      </c>
+      <c r="K463" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>88</v>
+      </c>
+      <c r="B464" t="s">
+        <v>19</v>
+      </c>
+      <c r="C464" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D464" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F464" t="s">
+        <v>40</v>
+      </c>
+      <c r="K464" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>92</v>
+      </c>
+      <c r="B465" t="s">
+        <v>19</v>
+      </c>
+      <c r="C465" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D465" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F465" t="s">
+        <v>40</v>
+      </c>
+      <c r="K465" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="466" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>72</v>
+      </c>
+      <c r="B466" t="s">
+        <v>19</v>
+      </c>
+      <c r="C466" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D466" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F466" t="s">
+        <v>40</v>
+      </c>
+      <c r="K466" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="467" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>75</v>
+      </c>
+      <c r="B467" t="s">
+        <v>19</v>
+      </c>
+      <c r="C467" s="2">
+        <v>43966</v>
+      </c>
+      <c r="D467" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F467" t="s">
+        <v>40</v>
+      </c>
+      <c r="K467" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>72</v>
+      </c>
+      <c r="B468" t="s">
+        <v>19</v>
+      </c>
+      <c r="C468" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D468" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F468" t="s">
+        <v>40</v>
+      </c>
+      <c r="K468" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="469" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>92</v>
+      </c>
+      <c r="B469" t="s">
+        <v>19</v>
+      </c>
+      <c r="C469" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D469" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F469" t="s">
+        <v>40</v>
+      </c>
+      <c r="K469" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>78</v>
+      </c>
+      <c r="B470" t="s">
+        <v>19</v>
+      </c>
+      <c r="C470" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D470" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F470" t="s">
+        <v>40</v>
+      </c>
+      <c r="K470" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>60</v>
+      </c>
+      <c r="B471" t="s">
+        <v>19</v>
+      </c>
+      <c r="C471" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D471" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F471" t="s">
+        <v>40</v>
+      </c>
+      <c r="K471" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="472" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>59</v>
+      </c>
+      <c r="B472" t="s">
+        <v>19</v>
+      </c>
+      <c r="C472" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D472" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F472" t="s">
+        <v>40</v>
+      </c>
+      <c r="K472" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="473" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>16</v>
+      </c>
+      <c r="B473" t="s">
+        <v>19</v>
+      </c>
+      <c r="C473" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D473" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F473" t="s">
+        <v>40</v>
+      </c>
+      <c r="K473" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="474" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>130</v>
+      </c>
+      <c r="B474" t="s">
+        <v>19</v>
+      </c>
+      <c r="C474" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D474" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F474" t="s">
+        <v>40</v>
+      </c>
+      <c r="K474" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="475" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>127</v>
+      </c>
+      <c r="B475" t="s">
+        <v>19</v>
+      </c>
+      <c r="C475" s="2">
+        <v>43969</v>
+      </c>
+      <c r="D475" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F475" t="s">
+        <v>40</v>
+      </c>
+      <c r="K475" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="476" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>84</v>
+      </c>
+      <c r="B476" t="s">
+        <v>19</v>
+      </c>
+      <c r="C476" s="2">
+        <v>43964</v>
+      </c>
+      <c r="D476" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F476" t="s">
+        <v>26</v>
+      </c>
+      <c r="K476" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="477" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>130</v>
+      </c>
+      <c r="B477" t="s">
+        <v>19</v>
+      </c>
+      <c r="C477" s="2">
+        <v>43964</v>
+      </c>
+      <c r="D477" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F477" t="s">
+        <v>26</v>
+      </c>
+      <c r="K477" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="478" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>79</v>
+      </c>
+      <c r="B478" t="s">
+        <v>19</v>
+      </c>
+      <c r="C478" s="2">
+        <v>43964</v>
+      </c>
+      <c r="D478" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F478" t="s">
+        <v>26</v>
+      </c>
+      <c r="K478" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="479" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>58</v>
+      </c>
+      <c r="B479" t="s">
+        <v>47</v>
+      </c>
+      <c r="C479" s="2">
+        <v>43967</v>
+      </c>
+      <c r="D479" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F479" t="s">
+        <v>26</v>
+      </c>
+      <c r="K479" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="480" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>89</v>
+      </c>
+      <c r="B480" t="s">
+        <v>19</v>
+      </c>
+      <c r="C480" s="2">
+        <v>43967</v>
+      </c>
+      <c r="D480" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F480" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="481" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A481" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B481" t="s">
+        <v>19</v>
+      </c>
+      <c r="C481" s="2">
+        <v>43953</v>
+      </c>
+      <c r="D481" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F481" t="s">
+        <v>26</v>
+      </c>
+      <c r="K481" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="482" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>75</v>
+      </c>
+      <c r="B482" t="s">
+        <v>19</v>
+      </c>
+      <c r="C482" s="2">
+        <v>43953</v>
+      </c>
+      <c r="D482" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F482" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>193</v>
+      </c>
+      <c r="B483" t="s">
+        <v>19</v>
+      </c>
+      <c r="C483" s="2">
+        <v>43951</v>
+      </c>
+      <c r="D483" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F483" t="s">
+        <v>26</v>
+      </c>
+      <c r="K483" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>84</v>
+      </c>
+      <c r="B484" t="s">
+        <v>19</v>
+      </c>
+      <c r="C484" s="2">
+        <v>43951</v>
+      </c>
+      <c r="D484" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F484" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="485" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>177</v>
+      </c>
+      <c r="B485" t="s">
+        <v>19</v>
+      </c>
+      <c r="C485" s="2">
+        <v>43951</v>
+      </c>
+      <c r="D485" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F485" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="486" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>32</v>
+      </c>
+      <c r="B486" t="s">
+        <v>19</v>
+      </c>
+      <c r="C486" s="2">
+        <v>43951</v>
+      </c>
+      <c r="D486" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F486" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="487" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>52</v>
+      </c>
+      <c r="B487" t="s">
+        <v>19</v>
+      </c>
+      <c r="C487" s="2">
+        <v>43951</v>
+      </c>
+      <c r="D487" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F487" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>35</v>
+      </c>
+      <c r="B488" t="s">
+        <v>19</v>
+      </c>
+      <c r="C488" s="2">
+        <v>43951</v>
+      </c>
+      <c r="D488" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F488" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A336" xr:uid="{C7E5F994-3E21-47C1-9550-D67738D7F487}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
+  <sortState ref="A2:J11">
     <sortCondition ref="C2:C11"/>
     <sortCondition ref="D2:D11"/>
   </sortState>
@@ -10976,24 +11608,24 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Updating observations 2020 is complete from A Botanist's Field Notes
</commit_message>
<xml_diff>
--- a/data/auralObservations.xlsx
+++ b/data/auralObservations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahipp\Documents\CODE\auralLandscapes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42CCDDF-B82C-473A-BA64-AC8E9D5BEFBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38D0BD9-B830-4398-A956-89ECD4D0306C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2115" windowWidth="10800" windowHeight="7830" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="200">
   <si>
     <t>taxon</t>
   </si>
@@ -611,6 +611,24 @@
   </si>
   <si>
     <t>chimney swift</t>
+  </si>
+  <si>
+    <t>time unspecified, but after the news</t>
+  </si>
+  <si>
+    <t>time unspecified, but hot afternoon</t>
+  </si>
+  <si>
+    <t>bracketing… "By a few days later, the trees purred with cicadas, and as I write this on the 12th of June, they still do. Each morning, Brooklyn and I walk through town beneath a cloud of murmurs and humming, as the cicadas gear up for the noisy day."</t>
+  </si>
+  <si>
+    <t>time unspecified, but morning moss work with Wayne</t>
+  </si>
+  <si>
+    <t>times estimated</t>
+  </si>
+  <si>
+    <t>purely a placeholder: the cranes streamed by all day</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830C5A1-1504-4FB4-98E5-D787D6C4A5A6}">
-  <dimension ref="A1:K488"/>
+  <dimension ref="A1:K511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C485" sqref="C485"/>
+    <sheetView tabSelected="1" topLeftCell="A480" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A504" sqref="A504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11583,6 +11601,433 @@
       </c>
       <c r="F488" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>75</v>
+      </c>
+      <c r="B489" t="s">
+        <v>19</v>
+      </c>
+      <c r="C489" s="2">
+        <v>44006</v>
+      </c>
+      <c r="D489" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F489" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="490" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>58</v>
+      </c>
+      <c r="B490" t="s">
+        <v>47</v>
+      </c>
+      <c r="C490" s="2">
+        <v>44006</v>
+      </c>
+      <c r="D490" s="3">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="F490" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="491" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>72</v>
+      </c>
+      <c r="B491" t="s">
+        <v>19</v>
+      </c>
+      <c r="C491" s="2">
+        <v>44006</v>
+      </c>
+      <c r="D491" s="3">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="F491" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>36</v>
+      </c>
+      <c r="B492" t="s">
+        <v>19</v>
+      </c>
+      <c r="C492" s="2">
+        <v>44006</v>
+      </c>
+      <c r="D492" s="3">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="F492" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>72</v>
+      </c>
+      <c r="B493" t="s">
+        <v>19</v>
+      </c>
+      <c r="C493" s="2">
+        <v>43979</v>
+      </c>
+      <c r="D493" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F493" t="s">
+        <v>26</v>
+      </c>
+      <c r="K493" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="494" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>75</v>
+      </c>
+      <c r="B494" t="s">
+        <v>19</v>
+      </c>
+      <c r="C494" s="2">
+        <v>43980</v>
+      </c>
+      <c r="D494" s="3">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F494" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="495" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>71</v>
+      </c>
+      <c r="B495" t="s">
+        <v>19</v>
+      </c>
+      <c r="C495" s="2">
+        <v>43980</v>
+      </c>
+      <c r="D495" s="3">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="F495" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>143</v>
+      </c>
+      <c r="B496" t="s">
+        <v>22</v>
+      </c>
+      <c r="C496" s="2">
+        <v>43984</v>
+      </c>
+      <c r="D496" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F496" t="s">
+        <v>111</v>
+      </c>
+      <c r="K496" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="497" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>143</v>
+      </c>
+      <c r="B497" t="s">
+        <v>22</v>
+      </c>
+      <c r="C497" s="2">
+        <v>43994</v>
+      </c>
+      <c r="D497" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F497" t="s">
+        <v>111</v>
+      </c>
+      <c r="K497" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="498" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>143</v>
+      </c>
+      <c r="B498" t="s">
+        <v>22</v>
+      </c>
+      <c r="C498" s="2">
+        <v>44024</v>
+      </c>
+      <c r="D498" s="3">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="F498" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="499" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>11</v>
+      </c>
+      <c r="B499" t="s">
+        <v>19</v>
+      </c>
+      <c r="C499" s="2">
+        <v>44128</v>
+      </c>
+      <c r="D499" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F499" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="500" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>113</v>
+      </c>
+      <c r="B500" t="s">
+        <v>19</v>
+      </c>
+      <c r="C500" s="2">
+        <v>44128</v>
+      </c>
+      <c r="D500" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F500" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="501" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>7</v>
+      </c>
+      <c r="B501" t="s">
+        <v>19</v>
+      </c>
+      <c r="C501" s="2">
+        <v>44049</v>
+      </c>
+      <c r="D501" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F501" t="s">
+        <v>40</v>
+      </c>
+      <c r="K501" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="502" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>72</v>
+      </c>
+      <c r="B502" t="s">
+        <v>19</v>
+      </c>
+      <c r="C502" s="2">
+        <v>44049</v>
+      </c>
+      <c r="D502" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F502" t="s">
+        <v>40</v>
+      </c>
+      <c r="K502" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="503" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>13</v>
+      </c>
+      <c r="B503" t="s">
+        <v>19</v>
+      </c>
+      <c r="C503" s="2">
+        <v>44050</v>
+      </c>
+      <c r="D503" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F503" t="s">
+        <v>26</v>
+      </c>
+      <c r="K503" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="504" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>71</v>
+      </c>
+      <c r="B504" t="s">
+        <v>19</v>
+      </c>
+      <c r="C504" s="2">
+        <v>44050</v>
+      </c>
+      <c r="D504" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F504" t="s">
+        <v>26</v>
+      </c>
+      <c r="K504" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="505" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>17</v>
+      </c>
+      <c r="B505" t="s">
+        <v>19</v>
+      </c>
+      <c r="C505" s="2">
+        <v>44050</v>
+      </c>
+      <c r="D505" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="F505" t="s">
+        <v>26</v>
+      </c>
+      <c r="K505" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="506" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>7</v>
+      </c>
+      <c r="B506" t="s">
+        <v>19</v>
+      </c>
+      <c r="C506" s="2">
+        <v>44056</v>
+      </c>
+      <c r="D506" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F506" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="507" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>11</v>
+      </c>
+      <c r="B507" t="s">
+        <v>19</v>
+      </c>
+      <c r="C507" s="2">
+        <v>44056</v>
+      </c>
+      <c r="D507" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F507" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="508" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>49</v>
+      </c>
+      <c r="B508" t="s">
+        <v>19</v>
+      </c>
+      <c r="C508" s="2">
+        <v>44144</v>
+      </c>
+      <c r="D508" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F508" t="s">
+        <v>40</v>
+      </c>
+      <c r="K508" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="509" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>98</v>
+      </c>
+      <c r="B509" t="s">
+        <v>19</v>
+      </c>
+      <c r="C509" s="2">
+        <v>44146</v>
+      </c>
+      <c r="D509" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F509" t="s">
+        <v>111</v>
+      </c>
+      <c r="K509" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="510" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>154</v>
+      </c>
+      <c r="B510" t="s">
+        <v>19</v>
+      </c>
+      <c r="C510" s="2">
+        <v>44146</v>
+      </c>
+      <c r="D510" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F510" t="s">
+        <v>111</v>
+      </c>
+      <c r="K510" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="511" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>101</v>
+      </c>
+      <c r="B511" t="s">
+        <v>19</v>
+      </c>
+      <c r="C511" s="2">
+        <v>44156</v>
+      </c>
+      <c r="D511" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F511" t="s">
+        <v>111</v>
+      </c>
+      <c r="K511" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding december owl to observations Otis avenue, a pair of owls calling, either side of house
</commit_message>
<xml_diff>
--- a/data/auralObservations.xlsx
+++ b/data/auralObservations.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\code\auralLandscapes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F1CB3A-9F39-4A29-A766-107CE7514D5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EA6622-3C6C-4479-8800-6CD91DB1FEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{FC8E283B-D15F-4A14-9FD2-F23A4F60CEBF}"/>
   </bookViews>
   <sheets>
     <sheet name="observations" sheetId="1" r:id="rId1"/>
     <sheet name="reviewedPosts" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">observations!$A$1:$A$336</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">observations!$A$1:$A$513</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2519" uniqueCount="200">
   <si>
     <t>taxon</t>
   </si>
@@ -1016,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5830C5A1-1504-4FB4-98E5-D787D6C4A5A6}">
-  <dimension ref="A1:K512"/>
+  <dimension ref="A1:K513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A458" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F504" sqref="F504:F512"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A273" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -12656,6 +12656,26 @@
         <v>9</v>
       </c>
       <c r="J512" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="513" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A513" t="s">
+        <v>11</v>
+      </c>
+      <c r="B513" t="s">
+        <v>19</v>
+      </c>
+      <c r="C513" s="2">
+        <v>44534</v>
+      </c>
+      <c r="D513" s="3">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="F513" t="s">
+        <v>9</v>
+      </c>
+      <c r="J513" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>